<commit_message>
updated data and Kubas photo
</commit_message>
<xml_diff>
--- a/data/seuk_04.xlsx
+++ b/data/seuk_04.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="14">
   <si>
     <t xml:space="preserve">﻿Date</t>
   </si>
@@ -178,10 +178,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M56" activeCellId="0" sqref="M56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K70" activeCellId="0" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>45022</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
         <v>45022</v>
       </c>
@@ -1787,10 +1787,440 @@
         <f aca="false">IF(F59&gt;G59,1,2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <f aca="false">IF(F60&gt;G60,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <f aca="false">IF(F61&gt;G61,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <f aca="false">IF(F62&gt;G62,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <f aca="false">IF(F63&gt;G63,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <f aca="false">IF(F64&gt;G64,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <f aca="false">IF(F65&gt;G65,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <f aca="false">IF(F66&gt;G66,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <f aca="false">IF(F67&gt;G67,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <f aca="false">IF(F68&gt;G68,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <f aca="false">IF(F69&gt;G69,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <f aca="false">IF(F70&gt;G70,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <f aca="false">IF(F71&gt;G71,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <f aca="false">IF(F72&gt;G72,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <f aca="false">IF(F73&gt;G73,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <f aca="false">IF(F74&gt;G74,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <f aca="false">IF(F75&gt;G75,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added env.yml and updated data
</commit_message>
<xml_diff>
--- a/data/seuk_04.xlsx
+++ b/data/seuk_04.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="14">
   <si>
     <t xml:space="preserve">﻿Date</t>
   </si>
@@ -178,10 +178,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O166"/>
+  <dimension ref="A1:O170"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I153" activeCellId="0" sqref="I153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M159" activeCellId="0" sqref="M159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4192,24 +4192,600 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E149" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <f aca="false">IF(F149&gt;G149,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <f aca="false">IF(F150&gt;G150,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <f aca="false">IF(F151&gt;G151,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <f aca="false">IF(F152&gt;G152,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <f aca="false">IF(F153&gt;G153,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <f aca="false">IF(F154&gt;G154,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <f aca="false">IF(F155&gt;G155,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <f aca="false">IF(F156&gt;G156,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E157" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <f aca="false">IF(F157&gt;G157,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <f aca="false">IF(F158&gt;G158,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D159" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G159" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <f aca="false">IF(F159&gt;G159,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G160" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H160" s="0" t="n">
+        <f aca="false">IF(F160&gt;G160,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C161" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D161" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E161" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G161" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <f aca="false">IF(F161&gt;G161,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G162" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H162" s="0" t="n">
+        <f aca="false">IF(F162&gt;G162,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C163" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E163" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G163" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H163" s="0" t="n">
+        <f aca="false">IF(F163&gt;G163,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G164" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H164" s="0" t="n">
+        <f aca="false">IF(F164&gt;G164,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <f aca="false">IF(F165&gt;G165,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <f aca="false">IF(F166&gt;G166,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E167" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <f aca="false">IF(F167&gt;G167,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <f aca="false">IF(F168&gt;G168,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <f aca="false">IF(F169&gt;G169,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <f aca="false">IF(F170&gt;G170,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>